<commit_message>
Agrego correcciones sobre el informe
</commit_message>
<xml_diff>
--- a/Tabla Reas.xlsx
+++ b/Tabla Reas.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FACULTAD\Inteligencia Artificial I\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Compartida\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927E8402-195B-4885-9014-74F0EB04A171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{09C881B9-5A8E-475B-B582-E3D6A7B9D6B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -201,7 +200,146 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: identificar la mayor cantidad de piezas posibles.
+      <t xml:space="preserve">: set de fotografía, con iluminacion controlada. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Audio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: sala de grabación, con el menor ruido posible. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Visión</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: cámara de celular, sin filtros ni efectos. Set con iluminacion uniforme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Audio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: micrófono de celular</t>
+    </r>
+  </si>
+  <si>
+    <t>Actuadores</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Versión actua</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">l: pantalla de la computadora. Ésta solo interactúa con el entorno mostrando los resultados del agente
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Potenciales actuadores</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: en el caso de implementar este agente en un entorno industrial real. En ese caso podríamos tener un brazo robótico que tenga un gripper para seleccionar las piezas. El brazo también tendrá la cámara para tomar las imágenes. El sistema dispondrá también de un sistema de grabación de comandos de voz.
+ </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Visión</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: identificar correctamente las piezas muestreadas.
 </t>
     </r>
     <r>
@@ -247,173 +385,12 @@
       </rPr>
       <t xml:space="preserve">: determinar la caja de origen mas probable </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Visión</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: set de fotografía, con iluminacion controlada. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Audio</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: sala de grabación, con el menor ruido posible. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Visión</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: cámara de celular, sin filtros ni efectos. Set con iluminacion uniforme
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Audio</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: micrófono de celular</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Visión</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: clasificar piezas
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Audio</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: reconocer comando y ejecutar acción
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Bayes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: mostrar proporciones/contar</t>
-    </r>
-  </si>
-  <si>
-    <t>Actuadores/
-Acciones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -466,13 +443,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -787,20 +770,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E84AF5C-A335-490F-B7C5-E4B4812D867F}">
-  <dimension ref="D5:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A5:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:F9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="6" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="6" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
@@ -811,7 +794,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="4:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
@@ -819,10 +803,11 @@
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="4:6" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
@@ -830,21 +815,21 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="4:6" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="4:6" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
@@ -852,7 +837,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>